<commit_message>
added code for schedule planner import, file upload related
</commit_message>
<xml_diff>
--- a/Data/ScheduleImport_Test.xlsx
+++ b/Data/ScheduleImport_Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\WFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A3AC26C-8C89-435D-B78F-98792AC270F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E985B9E8-6B48-432C-8302-CA58A54113C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -418,7 +418,7 @@
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>